<commit_message>
addresses #341 update checklist for OWASP ASVS Level 1 security check
</commit_message>
<xml_diff>
--- a/others/OWASP_ASVS_Level1_CheckList/OWASP_ASVS_Level1_Checklist.xlsx
+++ b/others/OWASP_ASVS_Level1_CheckList/OWASP_ASVS_Level1_Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritamachado/switch-2017-g003/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritamachado/switch-2017-g003/others/OWASP_ASVS_Level1_CheckList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06367A13-BCB0-7546-A7C3-D493F502ADE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1916C501-3D3E-DF47-B39C-D3A6D523AF9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="291">
   <si>
     <t>Category</t>
   </si>
@@ -901,6 +901,21 @@
   </si>
   <si>
     <t>We have no such functionalities implemented. This security verification step is not applicable to Project Managment Application.</t>
+  </si>
+  <si>
+    <t>The ‘password forgotten’ functionality doens't exist.</t>
+  </si>
+  <si>
+    <t>The system does not disclose whether a username is valid or not. It is not possible to collect a set of valid usernames by interacting with the authentication mechanism of the application.</t>
+  </si>
+  <si>
+    <t>Account lockout mechanisms are used to mitigate brute force password guessing attacks. Still this functionality was not implemented for this application.</t>
+  </si>
+  <si>
+    <t>There are not default passwords in use for this application. All passwords in used were checked against the default password list (defaultpassword.com) provided by OWASP website.</t>
+  </si>
+  <si>
+    <t>Application is accessed using HTTPS  both in frontend and backend</t>
   </si>
 </sst>
 </file>
@@ -2548,8 +2563,8 @@
   <dimension ref="A1:AC998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3467,15 +3482,21 @@
         <v>1</v>
       </c>
       <c r="K22" s="83" t="s">
-        <v>274</v>
-      </c>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
+        <v>272</v>
+      </c>
+      <c r="L22" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="75" t="s">
+        <v>9</v>
+      </c>
       <c r="N22" s="74" t="str">
         <f>IF(L22="I","I",IF(ISNA(VLOOKUP(M22, 'Lookup Tables'!$B$16:$E$19, MATCH(L22, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)),"",VLOOKUP(M22, 'Lookup Tables'!$B$16:$E$19, MATCH(L22, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)))</f>
-        <v/>
-      </c>
-      <c r="O22" s="20"/>
+        <v>H</v>
+      </c>
+      <c r="O22" s="89" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="23" spans="1:15" ht="46" thickBot="1">
       <c r="A23">
@@ -3507,7 +3528,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="83" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L23" s="75"/>
       <c r="M23" s="75"/>
@@ -3515,9 +3536,11 @@
         <f>IF(L23="I","I",IF(ISNA(VLOOKUP(M23, 'Lookup Tables'!$B$16:$E$19, MATCH(L23, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)),"",VLOOKUP(M23, 'Lookup Tables'!$B$16:$E$19, MATCH(L23, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)))</f>
         <v/>
       </c>
-      <c r="O23" s="20"/>
-    </row>
-    <row r="24" spans="1:15" ht="31" thickBot="1">
+      <c r="O23" s="89" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="58" thickBot="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3547,17 +3570,23 @@
         <v>1</v>
       </c>
       <c r="K24" s="83" t="s">
-        <v>274</v>
-      </c>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
+        <v>272</v>
+      </c>
+      <c r="L24" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="M24" s="75" t="s">
+        <v>21</v>
+      </c>
       <c r="N24" s="74" t="str">
         <f>IF(L24="I","I",IF(ISNA(VLOOKUP(M24, 'Lookup Tables'!$B$16:$E$19, MATCH(L24, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)),"",VLOOKUP(M24, 'Lookup Tables'!$B$16:$E$19, MATCH(L24, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)))</f>
-        <v/>
-      </c>
-      <c r="O24" s="20"/>
-    </row>
-    <row r="25" spans="1:15" ht="46" thickBot="1">
+        <v>L</v>
+      </c>
+      <c r="O24" s="89" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="58" thickBot="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3587,17 +3616,23 @@
         <v>1</v>
       </c>
       <c r="K25" s="83" t="s">
-        <v>274</v>
-      </c>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
+        <v>272</v>
+      </c>
+      <c r="L25" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="75" t="s">
+        <v>9</v>
+      </c>
       <c r="N25" s="74" t="str">
         <f>IF(L25="I","I",IF(ISNA(VLOOKUP(M25, 'Lookup Tables'!$B$16:$E$19, MATCH(L25, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)),"",VLOOKUP(M25, 'Lookup Tables'!$B$16:$E$19, MATCH(L25, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)))</f>
-        <v/>
-      </c>
-      <c r="O25" s="20"/>
-    </row>
-    <row r="26" spans="1:15" ht="46" thickBot="1">
+        <v>H</v>
+      </c>
+      <c r="O25" s="89" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="58" thickBot="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3627,15 +3662,21 @@
         <v>1</v>
       </c>
       <c r="K26" s="83" t="s">
-        <v>274</v>
-      </c>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
+        <v>273</v>
+      </c>
+      <c r="L26" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="75" t="s">
+        <v>9</v>
+      </c>
       <c r="N26" s="74" t="str">
         <f>IF(L26="I","I",IF(ISNA(VLOOKUP(M26, 'Lookup Tables'!$B$16:$E$19, MATCH(L26, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)),"",VLOOKUP(M26, 'Lookup Tables'!$B$16:$E$19, MATCH(L26, 'Lookup Tables'!$B$16:$E$16, 0), FALSE)))</f>
-        <v/>
-      </c>
-      <c r="O26" s="20"/>
+        <v>H</v>
+      </c>
+      <c r="O26" s="89" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="46" hidden="1" thickBot="1">
       <c r="A27">

</xml_diff>

<commit_message>
#341 Fixed minor error in security checklist
</commit_message>
<xml_diff>
--- a/others/OWASP_ASVS_Level1_CheckList/OWASP_ASVS_Level1_Checklist.xlsx
+++ b/others/OWASP_ASVS_Level1_CheckList/OWASP_ASVS_Level1_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritamachado/switch-2017-g003/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana_m\Documents\switch-2017-g003\others\OWASP_ASVS_Level1_CheckList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06367A13-BCB0-7546-A7C3-D493F502ADE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFF6BA3-BA49-441C-8448-938831279FAE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Data" sheetId="2" r:id="rId1"/>
@@ -876,12 +876,6 @@
     <t>Further Checks</t>
   </si>
   <si>
-    <t>In frontEnd, an automated tool was used (Deepcheck) to analyze unused dependencies. Also, all components were visually check for their usefulness in the application. In the backend, SonarLint was used to check, in each class if all imports are nedded. Also, all classes were visually check for their usefulness in the application.</t>
-  </si>
-  <si>
-    <t>A highOrderComponent (RequiresAuth) is used to verify if the user is uthenticated before accessing any protected page.</t>
-  </si>
-  <si>
     <t>All RestControllers were manually verified for authentication access. Authentication verification was also doublechecked using POSTMAN requests and automated integration tests.</t>
   </si>
   <si>
@@ -891,9 +885,6 @@
     <t>Spring Security is a great tool which helps with many aspects of building of secure applications. Spring Security  helps address  Cross-Site Request Forgery (CSRF) issues  by providing support for generation and validation of tokens. mitigating CSRF attacks.</t>
   </si>
   <si>
-    <t xml:space="preserve">Password is encpripted and credentials are used to generate a token. No where in the application the passowrd is available. </t>
-  </si>
-  <si>
     <t>The database was taken offline and the application did not allow log in.</t>
   </si>
   <si>
@@ -901,6 +892,15 @@
   </si>
   <si>
     <t>We have no such functionalities implemented. This security verification step is not applicable to Project Managment Application.</t>
+  </si>
+  <si>
+    <t>In frontEnd, an automated tool was used (Deepcheck) to analyze unused dependencies. Also, all components were visually check for their usefulness in the application. In the backend, SonarLint was used to check, in each class if all imports are needed. Also, all classes were visually checked for their usefulness in the application.</t>
+  </si>
+  <si>
+    <t>A highOrderComponent (RequiresAuth) is used to verify if the user is authenticated before accessing any protected page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password is encripted and credentials are used to generate a token. Nowhere in the application the password is available. </t>
   </si>
 </sst>
 </file>
@@ -2118,8 +2118,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
+    <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2246,7 +2246,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2548,27 +2548,27 @@
   <dimension ref="A1:AC998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="46.5" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
-    <col min="5" max="7" width="9.5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="7" width="9.42578125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="8" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="96.1640625" customWidth="1"/>
-    <col min="16" max="29" width="8.83203125" customWidth="1"/>
+    <col min="15" max="15" width="96.140625" customWidth="1"/>
+    <col min="16" max="29" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="21" thickBot="1">
+    <row r="1" spans="1:29" ht="32.25" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2627,7 +2627,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="97" thickTop="1" thickBot="1">
+    <row r="2" spans="1:29" ht="114" thickTop="1" thickBot="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2670,10 +2670,10 @@
         <v>M</v>
       </c>
       <c r="O2" s="87" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="46" hidden="1" thickBot="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="60.75" hidden="1" thickBot="1">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="O3" s="14"/>
     </row>
-    <row r="4" spans="1:29" ht="31" hidden="1" thickBot="1">
+    <row r="4" spans="1:29" ht="30.75" hidden="1" thickBot="1">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="1:29" ht="46" hidden="1" thickBot="1">
+    <row r="5" spans="1:29" ht="45.75" hidden="1" thickBot="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:29" ht="61" hidden="1" thickBot="1">
+    <row r="6" spans="1:29" ht="60.75" hidden="1" thickBot="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="1:29" ht="76" hidden="1" thickBot="1">
+    <row r="7" spans="1:29" ht="75.75" hidden="1" thickBot="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="O7" s="14"/>
     </row>
-    <row r="8" spans="1:29" ht="46" hidden="1" thickBot="1">
+    <row r="8" spans="1:29" ht="45.75" hidden="1" thickBot="1">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="1:29" ht="46" hidden="1" thickBot="1">
+    <row r="9" spans="1:29" ht="60.75" hidden="1" thickBot="1">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="1:29" ht="46" hidden="1" thickBot="1">
+    <row r="10" spans="1:29" ht="60.75" hidden="1" thickBot="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="1:29" ht="31" hidden="1" thickBot="1">
+    <row r="11" spans="1:29" ht="45.75" hidden="1" thickBot="1">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="1:29" ht="46" hidden="1" thickBot="1">
+    <row r="12" spans="1:29" ht="45.75" hidden="1" thickBot="1">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="1:29" ht="46" thickBot="1">
+    <row r="13" spans="1:29" ht="45.75" thickBot="1">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3090,10 +3090,10 @@
         <v>H</v>
       </c>
       <c r="O13" s="87" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" ht="91" thickBot="1">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="105.75" thickBot="1">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3136,10 +3136,10 @@
         <v>H</v>
       </c>
       <c r="O14" s="89" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" ht="58" thickBot="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="57" thickBot="1">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3182,10 +3182,10 @@
         <v>M</v>
       </c>
       <c r="O15" s="87" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="39" thickBot="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="38.25" thickBot="1">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3228,10 +3228,10 @@
         <v>M</v>
       </c>
       <c r="O16" s="87" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="61" thickBot="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="60.75" thickBot="1">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3274,10 +3274,10 @@
         <v>M</v>
       </c>
       <c r="O17" s="87" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="76" thickBot="1">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="90.75" thickBot="1">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3316,10 +3316,10 @@
         <v/>
       </c>
       <c r="O18" s="87" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="46" thickBot="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="57" thickBot="1">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3358,10 +3358,10 @@
         <v/>
       </c>
       <c r="O19" s="87" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="61" hidden="1" thickBot="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="21" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="1:15" ht="61" thickBot="1">
+    <row r="22" spans="1:15" ht="60.75" thickBot="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="O22" s="20"/>
     </row>
-    <row r="23" spans="1:15" ht="46" thickBot="1">
+    <row r="23" spans="1:15" ht="60.75" thickBot="1">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="O23" s="20"/>
     </row>
-    <row r="24" spans="1:15" ht="31" thickBot="1">
+    <row r="24" spans="1:15" ht="45.75" thickBot="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="O24" s="20"/>
     </row>
-    <row r="25" spans="1:15" ht="46" thickBot="1">
+    <row r="25" spans="1:15" ht="60.75" thickBot="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="O25" s="20"/>
     </row>
-    <row r="26" spans="1:15" ht="46" thickBot="1">
+    <row r="26" spans="1:15" ht="45.75" thickBot="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="O26" s="20"/>
     </row>
-    <row r="27" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="27" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="O27" s="14"/>
     </row>
-    <row r="28" spans="1:15" ht="61" thickBot="1">
+    <row r="28" spans="1:15" ht="75.75" thickBot="1">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="O28" s="20"/>
     </row>
-    <row r="29" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="29" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="O29" s="14"/>
     </row>
-    <row r="30" spans="1:15" ht="61" thickBot="1">
+    <row r="30" spans="1:15" ht="75.75" thickBot="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="O30" s="20"/>
     </row>
-    <row r="31" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="31" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="O31" s="14"/>
     </row>
-    <row r="32" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="32" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="O32" s="14"/>
     </row>
-    <row r="33" spans="1:15" ht="31" thickBot="1">
+    <row r="33" spans="1:15" ht="45.75" thickBot="1">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="O33" s="20"/>
     </row>
-    <row r="34" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="34" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="O34" s="14"/>
     </row>
-    <row r="35" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="35" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="O35" s="14"/>
     </row>
-    <row r="36" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="36" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="O36" s="14"/>
     </row>
-    <row r="37" spans="1:15" ht="31" thickBot="1">
+    <row r="37" spans="1:15" ht="30.75" thickBot="1">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="O37" s="14"/>
     </row>
-    <row r="38" spans="1:15" ht="46" thickBot="1">
+    <row r="38" spans="1:15" ht="45.75" thickBot="1">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="O38" s="20"/>
     </row>
-    <row r="39" spans="1:15" ht="46" thickBot="1">
+    <row r="39" spans="1:15" ht="45.75" thickBot="1">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4139,7 +4139,7 @@
       </c>
       <c r="O39" s="14"/>
     </row>
-    <row r="40" spans="1:15" ht="17" thickBot="1">
+    <row r="40" spans="1:15" ht="30.75" thickBot="1">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="O40" s="14"/>
     </row>
-    <row r="41" spans="1:15" ht="31" thickBot="1">
+    <row r="41" spans="1:15" ht="30.75" thickBot="1">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="O41" s="14"/>
     </row>
-    <row r="42" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="42" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="O42" s="14"/>
     </row>
-    <row r="43" spans="1:15" ht="31" thickBot="1">
+    <row r="43" spans="1:15" ht="45.75" thickBot="1">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="O43" s="14"/>
     </row>
-    <row r="44" spans="1:15" ht="61" thickBot="1">
+    <row r="44" spans="1:15" ht="60.75" thickBot="1">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="O44" s="14"/>
     </row>
-    <row r="45" spans="1:15" ht="31" thickBot="1">
+    <row r="45" spans="1:15" ht="45.75" thickBot="1">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="O45" s="14"/>
     </row>
-    <row r="46" spans="1:15" ht="31" thickBot="1">
+    <row r="46" spans="1:15" ht="45.75" thickBot="1">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="O46" s="20"/>
     </row>
-    <row r="47" spans="1:15" ht="31" thickBot="1">
+    <row r="47" spans="1:15" ht="45.75" thickBot="1">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="O47" s="14"/>
     </row>
-    <row r="48" spans="1:15" ht="61" thickBot="1">
+    <row r="48" spans="1:15" ht="75.75" thickBot="1">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="O48" s="20"/>
     </row>
-    <row r="49" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="49" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="O49" s="14"/>
     </row>
-    <row r="50" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="50" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4571,7 +4571,7 @@
       </c>
       <c r="O50" s="14"/>
     </row>
-    <row r="51" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="51" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4607,7 +4607,7 @@
       </c>
       <c r="O51" s="14"/>
     </row>
-    <row r="52" spans="1:15" ht="76" thickBot="1">
+    <row r="52" spans="1:15" ht="90.75" thickBot="1">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="O52" s="14"/>
     </row>
-    <row r="53" spans="1:15" ht="61" thickBot="1">
+    <row r="53" spans="1:15" ht="75.75" thickBot="1">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="O53" s="14"/>
     </row>
-    <row r="54" spans="1:15" ht="76" thickBot="1">
+    <row r="54" spans="1:15" ht="75.75" thickBot="1">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4727,7 +4727,7 @@
       </c>
       <c r="O54" s="14"/>
     </row>
-    <row r="55" spans="1:15" ht="17" thickBot="1">
+    <row r="55" spans="1:15" ht="16.5" thickBot="1">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4767,7 +4767,7 @@
       </c>
       <c r="O55" s="14"/>
     </row>
-    <row r="56" spans="1:15" ht="31" thickBot="1">
+    <row r="56" spans="1:15" ht="45.75" thickBot="1">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="O56" s="14"/>
     </row>
-    <row r="57" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="57" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="O57" s="14"/>
     </row>
-    <row r="58" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="58" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4881,7 +4881,7 @@
       </c>
       <c r="O58" s="14"/>
     </row>
-    <row r="59" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="59" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="O59" s="14"/>
     </row>
-    <row r="60" spans="1:15" ht="46" thickBot="1">
+    <row r="60" spans="1:15" ht="45.75" thickBot="1">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="O60" s="14"/>
     </row>
-    <row r="61" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="61" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="O61" s="14"/>
     </row>
-    <row r="62" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="62" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="O62" s="14"/>
     </row>
-    <row r="63" spans="1:15" ht="46" thickBot="1">
+    <row r="63" spans="1:15" ht="60.75" thickBot="1">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="O63" s="14"/>
     </row>
-    <row r="64" spans="1:15" ht="46" thickBot="1">
+    <row r="64" spans="1:15" ht="45.75" thickBot="1">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="O64" s="14"/>
     </row>
-    <row r="65" spans="1:15" ht="31" thickBot="1">
+    <row r="65" spans="1:15" ht="30.75" thickBot="1">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="O65" s="14"/>
     </row>
-    <row r="66" spans="1:15" ht="31" thickBot="1">
+    <row r="66" spans="1:15" ht="30.75" thickBot="1">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="O66" s="14"/>
     </row>
-    <row r="67" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="67" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="O67" s="14"/>
     </row>
-    <row r="68" spans="1:15" ht="61" thickBot="1">
+    <row r="68" spans="1:15" ht="75.75" thickBot="1">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="O68" s="14"/>
     </row>
-    <row r="69" spans="1:15" ht="46" thickBot="1">
+    <row r="69" spans="1:15" ht="45.75" thickBot="1">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5311,7 +5311,7 @@
       </c>
       <c r="O69" s="14"/>
     </row>
-    <row r="70" spans="1:15" ht="46" thickBot="1">
+    <row r="70" spans="1:15" ht="45.75" thickBot="1">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="O70" s="14"/>
     </row>
-    <row r="71" spans="1:15" ht="46" thickBot="1">
+    <row r="71" spans="1:15" ht="45.75" thickBot="1">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5391,7 +5391,7 @@
       </c>
       <c r="O71" s="14"/>
     </row>
-    <row r="72" spans="1:15" ht="46" thickBot="1">
+    <row r="72" spans="1:15" ht="60.75" thickBot="1">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5431,7 +5431,7 @@
       </c>
       <c r="O72" s="14"/>
     </row>
-    <row r="73" spans="1:15" ht="91" thickBot="1">
+    <row r="73" spans="1:15" ht="105.75" thickBot="1">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="O73" s="14"/>
     </row>
-    <row r="74" spans="1:15" ht="91" hidden="1" thickBot="1">
+    <row r="74" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5509,7 +5509,7 @@
       </c>
       <c r="O74" s="14"/>
     </row>
-    <row r="75" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="75" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="O75" s="14"/>
     </row>
-    <row r="76" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="76" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5585,7 +5585,7 @@
       </c>
       <c r="O76" s="14"/>
     </row>
-    <row r="77" spans="1:15" ht="91" hidden="1" thickBot="1">
+    <row r="77" spans="1:15" ht="105.75" hidden="1" thickBot="1">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5623,7 +5623,7 @@
       </c>
       <c r="O77" s="14"/>
     </row>
-    <row r="78" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="78" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5661,7 +5661,7 @@
       </c>
       <c r="O78" s="14"/>
     </row>
-    <row r="79" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="79" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="O79" s="14"/>
     </row>
-    <row r="80" spans="1:15" ht="61" thickBot="1">
+    <row r="80" spans="1:15" ht="75.75" thickBot="1">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5739,7 +5739,7 @@
       </c>
       <c r="O80" s="14"/>
     </row>
-    <row r="81" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="81" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="O81" s="14"/>
     </row>
-    <row r="82" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="82" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5815,7 +5815,7 @@
       </c>
       <c r="O82" s="14"/>
     </row>
-    <row r="83" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="83" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="O83" s="14"/>
     </row>
-    <row r="84" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="84" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5891,7 +5891,7 @@
       </c>
       <c r="O84" s="14"/>
     </row>
-    <row r="85" spans="1:15" ht="46" thickBot="1">
+    <row r="85" spans="1:15" ht="45.75" thickBot="1">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="O85" s="14"/>
     </row>
-    <row r="86" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="86" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="O86" s="14"/>
     </row>
-    <row r="87" spans="1:15" ht="46" thickBot="1">
+    <row r="87" spans="1:15" ht="45.75" thickBot="1">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="O87" s="14"/>
     </row>
-    <row r="88" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="88" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="O88" s="14"/>
     </row>
-    <row r="89" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="89" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6083,7 +6083,7 @@
       </c>
       <c r="O89" s="14"/>
     </row>
-    <row r="90" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="90" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="O90" s="14"/>
     </row>
-    <row r="91" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="91" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="O91" s="14"/>
     </row>
-    <row r="92" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="92" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6195,7 +6195,7 @@
       </c>
       <c r="O92" s="14"/>
     </row>
-    <row r="93" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="93" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="O93" s="14"/>
     </row>
-    <row r="94" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="94" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="O94" s="14"/>
     </row>
-    <row r="95" spans="1:15" ht="61" thickBot="1">
+    <row r="95" spans="1:15" ht="75.75" thickBot="1">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="O95" s="14"/>
     </row>
-    <row r="96" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="96" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="O96" s="14"/>
     </row>
-    <row r="97" spans="1:16" ht="46" hidden="1" thickBot="1">
+    <row r="97" spans="1:16" ht="45.75" hidden="1" thickBot="1">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="O97" s="14"/>
     </row>
-    <row r="98" spans="1:16" ht="46" hidden="1" thickBot="1">
+    <row r="98" spans="1:16" ht="60.75" hidden="1" thickBot="1">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6423,7 +6423,7 @@
       </c>
       <c r="O98" s="14"/>
     </row>
-    <row r="99" spans="1:16" ht="31" hidden="1" thickBot="1">
+    <row r="99" spans="1:16" ht="45.75" hidden="1" thickBot="1">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6461,7 +6461,7 @@
       </c>
       <c r="O99" s="14"/>
     </row>
-    <row r="100" spans="1:16" ht="31" hidden="1" thickBot="1">
+    <row r="100" spans="1:16" ht="30.75" hidden="1" thickBot="1">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="O100" s="14"/>
     </row>
-    <row r="101" spans="1:16" ht="91" hidden="1" thickBot="1">
+    <row r="101" spans="1:16" ht="105.75" hidden="1" thickBot="1">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6537,7 +6537,7 @@
       </c>
       <c r="O101" s="14"/>
     </row>
-    <row r="102" spans="1:16" ht="46" hidden="1" thickBot="1">
+    <row r="102" spans="1:16" ht="45.75" hidden="1" thickBot="1">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6573,7 +6573,7 @@
       </c>
       <c r="O102" s="14"/>
     </row>
-    <row r="103" spans="1:16" ht="31" hidden="1" thickBot="1">
+    <row r="103" spans="1:16" ht="30.75" hidden="1" thickBot="1">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6609,7 +6609,7 @@
       </c>
       <c r="O103" s="14"/>
     </row>
-    <row r="104" spans="1:16" ht="31" thickBot="1">
+    <row r="104" spans="1:16" ht="30.75" thickBot="1">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6649,7 +6649,7 @@
       </c>
       <c r="O104" s="14"/>
     </row>
-    <row r="105" spans="1:16" ht="46" hidden="1" thickBot="1">
+    <row r="105" spans="1:16" ht="45.75" hidden="1" thickBot="1">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="O105" s="14"/>
     </row>
-    <row r="106" spans="1:16" ht="31" hidden="1" thickBot="1">
+    <row r="106" spans="1:16" ht="45.75" hidden="1" thickBot="1">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6721,7 +6721,7 @@
       </c>
       <c r="O106" s="14"/>
     </row>
-    <row r="107" spans="1:16" ht="31" thickBot="1">
+    <row r="107" spans="1:16" ht="30.75" thickBot="1">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6762,7 +6762,7 @@
       <c r="O107" s="14"/>
       <c r="P107" s="13"/>
     </row>
-    <row r="108" spans="1:16" ht="46" thickBot="1">
+    <row r="108" spans="1:16" ht="45.75" thickBot="1">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6802,7 +6802,7 @@
       </c>
       <c r="O108" s="14"/>
     </row>
-    <row r="109" spans="1:16" ht="76" hidden="1" thickBot="1">
+    <row r="109" spans="1:16" ht="75.75" hidden="1" thickBot="1">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="O109" s="14"/>
     </row>
-    <row r="110" spans="1:16" ht="46" thickBot="1">
+    <row r="110" spans="1:16" ht="60.75" thickBot="1">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6878,7 +6878,7 @@
       </c>
       <c r="O110" s="14"/>
     </row>
-    <row r="111" spans="1:16" ht="76" thickBot="1">
+    <row r="111" spans="1:16" ht="90.75" thickBot="1">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="O111" s="14"/>
     </row>
-    <row r="112" spans="1:16" ht="61" hidden="1" thickBot="1">
+    <row r="112" spans="1:16" ht="75.75" hidden="1" thickBot="1">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6956,7 +6956,7 @@
       </c>
       <c r="O112" s="14"/>
     </row>
-    <row r="113" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="113" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="O113" s="14"/>
     </row>
-    <row r="114" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="114" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="O114" s="14"/>
     </row>
-    <row r="115" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="115" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A115">
         <v>114</v>
       </c>
@@ -7066,7 +7066,7 @@
       </c>
       <c r="O115" s="14"/>
     </row>
-    <row r="116" spans="1:15" ht="61" thickBot="1">
+    <row r="116" spans="1:15" ht="60.75" thickBot="1">
       <c r="A116">
         <v>115</v>
       </c>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="O116" s="14"/>
     </row>
-    <row r="117" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="117" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A117">
         <v>116</v>
       </c>
@@ -7144,7 +7144,7 @@
       </c>
       <c r="O117" s="14"/>
     </row>
-    <row r="118" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="118" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7182,7 +7182,7 @@
       </c>
       <c r="O118" s="14"/>
     </row>
-    <row r="119" spans="1:15" ht="46" thickBot="1">
+    <row r="119" spans="1:15" ht="60.75" thickBot="1">
       <c r="A119">
         <v>118</v>
       </c>
@@ -7222,7 +7222,7 @@
       </c>
       <c r="O119" s="14"/>
     </row>
-    <row r="120" spans="1:15" ht="76" thickBot="1">
+    <row r="120" spans="1:15" ht="105.75" thickBot="1">
       <c r="A120">
         <v>119</v>
       </c>
@@ -7262,7 +7262,7 @@
       </c>
       <c r="O120" s="14"/>
     </row>
-    <row r="121" spans="1:15" ht="17" hidden="1" thickBot="1">
+    <row r="121" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A121">
         <v>120</v>
       </c>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="O121" s="14"/>
     </row>
-    <row r="122" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="122" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="O122" s="14"/>
     </row>
-    <row r="123" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="123" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A123">
         <v>122</v>
       </c>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="O123" s="14"/>
     </row>
-    <row r="124" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="124" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7408,7 +7408,7 @@
       </c>
       <c r="O124" s="14"/>
     </row>
-    <row r="125" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="125" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7446,7 +7446,7 @@
       </c>
       <c r="O125" s="14"/>
     </row>
-    <row r="126" spans="1:15" ht="61" thickBot="1">
+    <row r="126" spans="1:15" ht="60.75" thickBot="1">
       <c r="A126">
         <v>125</v>
       </c>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="O126" s="14"/>
     </row>
-    <row r="127" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="127" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A127">
         <v>126</v>
       </c>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="O127" s="14"/>
     </row>
-    <row r="128" spans="1:15" ht="31" thickBot="1">
+    <row r="128" spans="1:15" ht="30.75" thickBot="1">
       <c r="A128">
         <v>127</v>
       </c>
@@ -7562,7 +7562,7 @@
       </c>
       <c r="O128" s="14"/>
     </row>
-    <row r="129" spans="1:15" ht="46" thickBot="1">
+    <row r="129" spans="1:15" ht="45.75" thickBot="1">
       <c r="A129">
         <v>128</v>
       </c>
@@ -7602,7 +7602,7 @@
       </c>
       <c r="O129" s="14"/>
     </row>
-    <row r="130" spans="1:15" ht="61" thickBot="1">
+    <row r="130" spans="1:15" ht="60.75" thickBot="1">
       <c r="A130">
         <v>129</v>
       </c>
@@ -7642,7 +7642,7 @@
       </c>
       <c r="O130" s="14"/>
     </row>
-    <row r="131" spans="1:15" ht="46" thickBot="1">
+    <row r="131" spans="1:15" ht="60.75" thickBot="1">
       <c r="A131">
         <v>130</v>
       </c>
@@ -7682,7 +7682,7 @@
       </c>
       <c r="O131" s="14"/>
     </row>
-    <row r="132" spans="1:15" ht="61" thickBot="1">
+    <row r="132" spans="1:15" ht="75.75" thickBot="1">
       <c r="A132">
         <v>131</v>
       </c>
@@ -7722,7 +7722,7 @@
       </c>
       <c r="O132" s="14"/>
     </row>
-    <row r="133" spans="1:15" ht="46" thickBot="1">
+    <row r="133" spans="1:15" ht="45.75" thickBot="1">
       <c r="A133">
         <v>132</v>
       </c>
@@ -7762,7 +7762,7 @@
       </c>
       <c r="O133" s="14"/>
     </row>
-    <row r="134" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="134" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A134">
         <v>133</v>
       </c>
@@ -7800,7 +7800,7 @@
       </c>
       <c r="O134" s="14"/>
     </row>
-    <row r="135" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="135" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A135">
         <v>134</v>
       </c>
@@ -7838,7 +7838,7 @@
       </c>
       <c r="O135" s="14"/>
     </row>
-    <row r="136" spans="1:15" ht="46" thickBot="1">
+    <row r="136" spans="1:15" ht="45.75" thickBot="1">
       <c r="A136">
         <v>135</v>
       </c>
@@ -7878,7 +7878,7 @@
       </c>
       <c r="O136" s="14"/>
     </row>
-    <row r="137" spans="1:15" ht="61" thickBot="1">
+    <row r="137" spans="1:15" ht="60.75" thickBot="1">
       <c r="A137">
         <v>136</v>
       </c>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="O137" s="14"/>
     </row>
-    <row r="138" spans="1:15" ht="46" thickBot="1">
+    <row r="138" spans="1:15" ht="45.75" thickBot="1">
       <c r="A138">
         <v>137</v>
       </c>
@@ -7958,7 +7958,7 @@
       </c>
       <c r="O138" s="14"/>
     </row>
-    <row r="139" spans="1:15" ht="31" thickBot="1">
+    <row r="139" spans="1:15" ht="45.75" thickBot="1">
       <c r="A139">
         <v>138</v>
       </c>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="O139" s="14"/>
     </row>
-    <row r="140" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="140" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8034,7 +8034,7 @@
       </c>
       <c r="O140" s="14"/>
     </row>
-    <row r="141" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="141" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8070,7 +8070,7 @@
       </c>
       <c r="O141" s="14"/>
     </row>
-    <row r="142" spans="1:15" ht="76" hidden="1" thickBot="1">
+    <row r="142" spans="1:15" ht="90.75" hidden="1" thickBot="1">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8108,7 +8108,7 @@
       </c>
       <c r="O142" s="14"/>
     </row>
-    <row r="143" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="143" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8146,7 +8146,7 @@
       </c>
       <c r="O143" s="14"/>
     </row>
-    <row r="144" spans="1:15" ht="46" thickBot="1">
+    <row r="144" spans="1:15" ht="60.75" thickBot="1">
       <c r="A144">
         <v>143</v>
       </c>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="O144" s="14"/>
     </row>
-    <row r="145" spans="1:15" ht="76" thickBot="1">
+    <row r="145" spans="1:15" ht="90.75" thickBot="1">
       <c r="A145">
         <v>144</v>
       </c>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="O145" s="14"/>
     </row>
-    <row r="146" spans="1:15" ht="46" thickBot="1">
+    <row r="146" spans="1:15" ht="60.75" thickBot="1">
       <c r="A146">
         <v>145</v>
       </c>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="O146" s="14"/>
     </row>
-    <row r="147" spans="1:15" ht="46" thickBot="1">
+    <row r="147" spans="1:15" ht="60.75" thickBot="1">
       <c r="A147">
         <v>146</v>
       </c>
@@ -8306,7 +8306,7 @@
       </c>
       <c r="O147" s="14"/>
     </row>
-    <row r="148" spans="1:15" ht="46" thickBot="1">
+    <row r="148" spans="1:15" ht="45.75" thickBot="1">
       <c r="A148">
         <v>147</v>
       </c>
@@ -8346,7 +8346,7 @@
       </c>
       <c r="O148" s="14"/>
     </row>
-    <row r="149" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="149" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A149">
         <v>148</v>
       </c>
@@ -8384,7 +8384,7 @@
       </c>
       <c r="O149" s="14"/>
     </row>
-    <row r="150" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="150" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A150">
         <v>149</v>
       </c>
@@ -8422,7 +8422,7 @@
       </c>
       <c r="O150" s="14"/>
     </row>
-    <row r="151" spans="1:15" ht="31" thickBot="1">
+    <row r="151" spans="1:15" ht="30.75" thickBot="1">
       <c r="A151">
         <v>150</v>
       </c>
@@ -8462,7 +8462,7 @@
       </c>
       <c r="O151" s="14"/>
     </row>
-    <row r="152" spans="1:15" ht="61" thickBot="1">
+    <row r="152" spans="1:15" ht="60.75" thickBot="1">
       <c r="A152">
         <v>151</v>
       </c>
@@ -8502,7 +8502,7 @@
       </c>
       <c r="O152" s="14"/>
     </row>
-    <row r="153" spans="1:15" ht="46" thickBot="1">
+    <row r="153" spans="1:15" ht="60.75" thickBot="1">
       <c r="A153">
         <v>152</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="46" thickBot="1">
+    <row r="154" spans="1:15" ht="60.75" thickBot="1">
       <c r="A154">
         <v>153</v>
       </c>
@@ -8586,7 +8586,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="31" thickBot="1">
+    <row r="155" spans="1:15" ht="45.75" thickBot="1">
       <c r="A155">
         <v>154</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="31" thickBot="1">
+    <row r="156" spans="1:15" ht="45.75" thickBot="1">
       <c r="A156">
         <v>155</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="157" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A157">
         <v>156</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="158" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A158">
         <v>157</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="31" thickBot="1">
+    <row r="159" spans="1:15" ht="30.75" thickBot="1">
       <c r="A159">
         <v>158</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="160" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A160">
         <v>159</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="46" thickBot="1">
+    <row r="161" spans="1:15" ht="45.75" thickBot="1">
       <c r="A161">
         <v>160</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="162" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A162">
         <v>161</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="31" thickBot="1">
+    <row r="163" spans="1:15" ht="30.75" thickBot="1">
       <c r="A163">
         <v>162</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="31" thickBot="1">
+    <row r="164" spans="1:15" ht="30.75" thickBot="1">
       <c r="A164">
         <v>165</v>
       </c>
@@ -8982,7 +8982,7 @@
       </c>
       <c r="O164" s="14"/>
     </row>
-    <row r="165" spans="1:15" ht="46" thickBot="1">
+    <row r="165" spans="1:15" ht="60.75" thickBot="1">
       <c r="A165">
         <v>166</v>
       </c>
@@ -9022,7 +9022,7 @@
       </c>
       <c r="O165" s="14"/>
     </row>
-    <row r="166" spans="1:15" ht="31" thickBot="1">
+    <row r="166" spans="1:15" ht="30.75" thickBot="1">
       <c r="A166">
         <v>167</v>
       </c>
@@ -9062,7 +9062,7 @@
       </c>
       <c r="O166" s="14"/>
     </row>
-    <row r="167" spans="1:15" ht="17" thickBot="1">
+    <row r="167" spans="1:15" ht="30.75" thickBot="1">
       <c r="A167">
         <v>168</v>
       </c>
@@ -9102,7 +9102,7 @@
       </c>
       <c r="O167" s="14"/>
     </row>
-    <row r="168" spans="1:15" ht="46" thickBot="1">
+    <row r="168" spans="1:15" ht="60.75" thickBot="1">
       <c r="A168">
         <v>169</v>
       </c>
@@ -9142,7 +9142,7 @@
       </c>
       <c r="O168" s="14"/>
     </row>
-    <row r="169" spans="1:15" ht="61" thickBot="1">
+    <row r="169" spans="1:15" ht="60.75" thickBot="1">
       <c r="A169">
         <v>170</v>
       </c>
@@ -9182,7 +9182,7 @@
       </c>
       <c r="O169" s="14"/>
     </row>
-    <row r="170" spans="1:15" ht="77" thickBot="1">
+    <row r="170" spans="1:15" ht="75.75" thickBot="1">
       <c r="A170">
         <v>171</v>
       </c>
@@ -9221,10 +9221,10 @@
         <v/>
       </c>
       <c r="O170" s="91" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="171" spans="1:15" ht="46" hidden="1" thickBot="1">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A171">
         <v>172</v>
       </c>
@@ -9261,7 +9261,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="172" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A172">
         <v>173</v>
       </c>
@@ -9298,10 +9298,10 @@
         <v/>
       </c>
       <c r="O172" s="90" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="173" spans="1:15" ht="31" hidden="1" thickBot="1">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A173">
         <v>174</v>
       </c>
@@ -9339,7 +9339,7 @@
       </c>
       <c r="O173" s="14"/>
     </row>
-    <row r="174" spans="1:15" ht="76" thickBot="1">
+    <row r="174" spans="1:15" ht="90.75" thickBot="1">
       <c r="A174">
         <v>175</v>
       </c>
@@ -9379,7 +9379,7 @@
       </c>
       <c r="O174" s="14"/>
     </row>
-    <row r="175" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="175" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A175">
         <v>176</v>
       </c>
@@ -9417,7 +9417,7 @@
       </c>
       <c r="O175" s="14"/>
     </row>
-    <row r="176" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="176" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A176">
         <v>177</v>
       </c>
@@ -9455,7 +9455,7 @@
       </c>
       <c r="O176" s="14"/>
     </row>
-    <row r="177" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="177" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A177">
         <v>178</v>
       </c>
@@ -9493,7 +9493,7 @@
       </c>
       <c r="O177" s="14"/>
     </row>
-    <row r="178" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="178" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A178">
         <v>179</v>
       </c>
@@ -9531,7 +9531,7 @@
       </c>
       <c r="O178" s="14"/>
     </row>
-    <row r="179" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="179" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A179">
         <v>180</v>
       </c>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="O179" s="14"/>
     </row>
-    <row r="180" spans="1:15" ht="17" hidden="1" thickBot="1">
+    <row r="180" spans="1:15" ht="16.5" hidden="1" thickBot="1">
       <c r="A180">
         <v>181</v>
       </c>
@@ -9603,7 +9603,7 @@
       </c>
       <c r="O180" s="14"/>
     </row>
-    <row r="181" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="181" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A181">
         <v>182</v>
       </c>
@@ -9639,7 +9639,7 @@
       </c>
       <c r="O181" s="14"/>
     </row>
-    <row r="182" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="182" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A182">
         <v>183</v>
       </c>
@@ -9675,7 +9675,7 @@
       </c>
       <c r="O182" s="14"/>
     </row>
-    <row r="183" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="183" spans="1:15" ht="75.75" hidden="1" thickBot="1">
       <c r="A183">
         <v>184</v>
       </c>
@@ -9711,7 +9711,7 @@
       </c>
       <c r="O183" s="14"/>
     </row>
-    <row r="184" spans="1:15" ht="61" hidden="1" thickBot="1">
+    <row r="184" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A184">
         <v>185</v>
       </c>
@@ -9749,7 +9749,7 @@
       </c>
       <c r="O184" s="14"/>
     </row>
-    <row r="185" spans="1:15" ht="31" thickBot="1">
+    <row r="185" spans="1:15" ht="30.75" thickBot="1">
       <c r="A185">
         <v>186</v>
       </c>
@@ -9791,7 +9791,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="31" thickBot="1">
+    <row r="186" spans="1:15" ht="30.75" thickBot="1">
       <c r="A186">
         <v>187</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="31" thickBot="1">
+    <row r="187" spans="1:15" ht="45.75" thickBot="1">
       <c r="A187">
         <v>188</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="46" thickBot="1">
+    <row r="188" spans="1:15" ht="60.75" thickBot="1">
       <c r="A188">
         <v>189</v>
       </c>
@@ -9917,7 +9917,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="31" thickBot="1">
+    <row r="189" spans="1:15" ht="30.75" thickBot="1">
       <c r="A189">
         <v>190</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="31" thickBot="1">
+    <row r="190" spans="1:15" ht="30.75" thickBot="1">
       <c r="A190">
         <v>191</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="31" thickBot="1">
+    <row r="191" spans="1:15" ht="30.75" thickBot="1">
       <c r="A191">
         <v>192</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="31" thickBot="1">
+    <row r="192" spans="1:15" ht="30.75" thickBot="1">
       <c r="A192">
         <v>193</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="31" thickBot="1">
+    <row r="193" spans="1:15" ht="30.75" thickBot="1">
       <c r="A193">
         <v>194</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="194" spans="1:15" ht="31" thickBot="1">
+    <row r="194" spans="1:15" ht="30.75" thickBot="1">
       <c r="A194">
         <v>195</v>
       </c>
@@ -10169,7 +10169,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="31" thickBot="1">
+    <row r="195" spans="1:15" ht="30.75" thickBot="1">
       <c r="A195">
         <v>196</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="196" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A196">
         <v>197</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="197" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A197">
         <v>198</v>
       </c>
@@ -10285,7 +10285,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="198" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A198">
         <v>199</v>
       </c>
@@ -10322,7 +10322,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="199" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A199">
         <v>200</v>
       </c>
@@ -10359,7 +10359,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="200" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A200">
         <v>201</v>
       </c>
@@ -10396,7 +10396,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="201" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A201">
         <v>202</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="202" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A202">
         <v>203</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="203" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A203">
         <v>204</v>
       </c>
@@ -10507,7 +10507,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="204" spans="1:15" ht="30.75" hidden="1" thickBot="1">
       <c r="A204">
         <v>205</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="205" spans="1:15" ht="60.75" hidden="1" thickBot="1">
       <c r="A205">
         <v>206</v>
       </c>
@@ -10581,7 +10581,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="206" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A206">
         <v>207</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="31" hidden="1" thickBot="1">
+    <row r="207" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A207">
         <v>208</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="46" hidden="1" thickBot="1">
+    <row r="208" spans="1:15" ht="45.75" hidden="1" thickBot="1">
       <c r="A208">
         <v>209</v>
       </c>
@@ -10686,7 +10686,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="31" hidden="1" thickBot="1">
+    <row r="209" spans="1:14" ht="30.75" hidden="1" thickBot="1">
       <c r="A209">
         <v>210</v>
       </c>
@@ -10721,7 +10721,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="17" hidden="1" thickBot="1">
+    <row r="210" spans="1:14" ht="30.75" hidden="1" thickBot="1">
       <c r="A210">
         <v>211</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="31" hidden="1" thickBot="1">
+    <row r="211" spans="1:14" ht="30.75" hidden="1" thickBot="1">
       <c r="A211">
         <v>212</v>
       </c>
@@ -10791,7 +10791,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="31" hidden="1" thickBot="1">
+    <row r="212" spans="1:14" ht="45.75" hidden="1" thickBot="1">
       <c r="A212">
         <v>213</v>
       </c>
@@ -10826,7 +10826,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="31" hidden="1" thickBot="1">
+    <row r="213" spans="1:14" ht="30.75" hidden="1" thickBot="1">
       <c r="A213">
         <v>214</v>
       </c>
@@ -17248,11 +17248,11 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="5" width="9.1640625" customWidth="1"/>
-    <col min="6" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>